<commit_message>
Datos Calentamiento y Enfriamiento del agua
</commit_message>
<xml_diff>
--- a/Cal y Enf Agua Datos.xlsx
+++ b/Cal y Enf Agua Datos.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecobu\Documents\Manuel Trabajos\UNI\6to\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC8CF91-4B06-4F09-813E-5F9F45F65689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A20D4E71-FAEF-405A-9991-1A146DBB8A6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Graficas" sheetId="1" r:id="rId1"/>
     <sheet name="Calculos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -132,9 +126,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -187,26 +181,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -265,8 +239,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -308,132 +281,108 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Calculos!$A$2:$A$19</c:f>
+              <c:f>Calculos!$A$4:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>240</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>360</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>480</c:v>
+                  <c:v>720</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600</c:v>
+                  <c:v>840</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>720</c:v>
+                  <c:v>960</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>840</c:v>
+                  <c:v>1080</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>960</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1080</c:v>
+                  <c:v>1320</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1200</c:v>
+                  <c:v>1440</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1320</c:v>
+                  <c:v>1560</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1440</c:v>
+                  <c:v>1680</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1560</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1680</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1920</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2040</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Calculos!$B$2:$B$19</c:f>
+              <c:f>Calculos!$B$4:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>61</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>67</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>77</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>81</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>84</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>86</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0ACD-4BED-B777-0F2065C283F1}"/>
             </c:ext>
@@ -447,11 +396,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="843380000"/>
-        <c:axId val="852645888"/>
+        <c:axId val="197805184"/>
+        <c:axId val="197806720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="843380000"/>
+        <c:axId val="197805184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,12 +457,12 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="852645888"/>
+        <c:crossAx val="197806720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="852645888"/>
+        <c:axId val="197806720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -570,7 +519,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="843380000"/>
+        <c:crossAx val="197805184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -584,14 +533,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -627,9 +576,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -641,6 +590,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -737,15 +687,14 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="exp"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.15956517935258094"/>
-                  <c:y val="-0.43952865266841645"/>
+                  <c:x val="3.9584761402054976E-2"/>
+                  <c:y val="-0.18310776370345011"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -780,50 +729,47 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Calculos!$A$24:$A$37</c:f>
+              <c:f>Calculos!$A$25:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>240</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>360</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>480</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600</c:v>
+                  <c:v>720</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>720</c:v>
+                  <c:v>840</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>840</c:v>
+                  <c:v>960</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>960</c:v>
+                  <c:v>1080</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1080</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1200</c:v>
+                  <c:v>1320</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1320</c:v>
+                  <c:v>1440</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1440</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>1560</c:v>
                 </c:pt>
               </c:numCache>
@@ -831,57 +777,54 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Calculos!$B$24:$B$37</c:f>
+              <c:f>Calculos!$B$25:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>91</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>72</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>68</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>65</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>62</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>59</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>57</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-674C-494C-BB3F-01C03F6735E6}"/>
             </c:ext>
@@ -895,11 +838,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1420969696"/>
-        <c:axId val="756853760"/>
+        <c:axId val="197849856"/>
+        <c:axId val="197851392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1420969696"/>
+        <c:axId val="197849856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,12 +899,12 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="756853760"/>
+        <c:crossAx val="197851392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="756853760"/>
+        <c:axId val="197851392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1018,7 +961,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1420969696"/>
+        <c:crossAx val="197849856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1032,14 +975,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1075,9 +1018,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1089,6 +1032,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1161,8 +1105,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="exp"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1293,7 +1236,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F99D-456F-ABDB-AE359A4F268B}"/>
             </c:ext>
@@ -1307,11 +1250,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1376928560"/>
-        <c:axId val="1433299728"/>
+        <c:axId val="198282624"/>
+        <c:axId val="198292608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1376928560"/>
+        <c:axId val="198282624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1368,12 +1311,12 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1433299728"/>
+        <c:crossAx val="198292608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1433299728"/>
+        <c:axId val="198292608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1373,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1376928560"/>
+        <c:crossAx val="198282624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1444,14 +1387,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1487,9 +1430,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1501,6 +1444,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1744,7 +1688,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-415B-4DC0-BDB5-4163F8D1D335}"/>
             </c:ext>
@@ -1958,7 +1902,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-415B-4DC0-BDB5-4163F8D1D335}"/>
             </c:ext>
@@ -1972,11 +1916,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1376242880"/>
-        <c:axId val="852654048"/>
+        <c:axId val="198383872"/>
+        <c:axId val="198390144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1376242880"/>
+        <c:axId val="198383872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2033,12 +1977,12 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="852654048"/>
+        <c:crossAx val="198390144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="852654048"/>
+        <c:axId val="198390144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2095,7 +2039,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1376242880"/>
+        <c:crossAx val="198383872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2109,6 +2053,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2140,14 +2085,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2182,2230 +2127,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -4426,7 +2147,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD6C802A-6A0B-B559-6DBF-D277EEDB3BF6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AD6C802A-6A0B-B559-6DBF-D277EEDB3BF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4485,7 +2206,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C020B987-78D9-3FBB-35B8-A9819E562D67}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C020B987-78D9-3FBB-35B8-A9819E562D67}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4544,7 +2265,7 @@
         <xdr:cNvPr id="5" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC9DDC48-1C17-48FE-5E3C-6A3439DA10FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BC9DDC48-1C17-48FE-5E3C-6A3439DA10FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4603,7 +2324,7 @@
         <xdr:cNvPr id="6" name="Imagen 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B913B78D-B8F0-336D-43B1-2965750AFD02}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B913B78D-B8F0-336D-43B1-2965750AFD02}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4667,7 +2388,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8229BCB0-A784-0354-EC12-7385CB2E41E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8229BCB0-A784-0354-EC12-7385CB2E41E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4690,20 +2411,20 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{725D54DE-5291-977C-3B4A-67976D21C80B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{725D54DE-5291-977C-3B4A-67976D21C80B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4739,7 +2460,7 @@
         <xdr:cNvPr id="5" name="Gráfico 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4751288A-58BF-9B75-EAAC-49E67BBFD84F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4751288A-58BF-9B75-EAAC-49E67BBFD84F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4775,7 +2496,7 @@
         <xdr:cNvPr id="6" name="Gráfico 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3F01CB4-1B94-3813-8A5E-83776BB0D6F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D3F01CB4-1B94-3813-8A5E-83776BB0D6F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4839,7 +2560,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4891,7 +2612,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5085,17 +2806,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6033F931-57B4-47B1-9067-77BE6857365B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
@@ -5107,11 +2828,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBE4415-23B3-4C88-995C-7332BF06AB77}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>